<commit_message>
made the departments table
</commit_message>
<xml_diff>
--- a/sponsored_2018.xlsx
+++ b/sponsored_2018.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Norman\Desktop\zagsabroad\zags-abroad-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3257CFCE-5E34-48B8-81EA-0643842ACCC9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF4709-16F2-4EA5-AF6D-3DE9F00451C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11003" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="7035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL EQUIVALENCIES use Filter " sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL EQUIVALENCIES use Filter '!$K$1:$K$1447</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -11326,8 +11329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C322" sqref="C322"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -56794,6 +56797,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K1:K1447" xr:uid="{6DD63BD1-B5FC-4FFB-AEE6-8F2876966816}"/>
   <sortState ref="A1:K1645">
     <sortCondition ref="A1:A1645"/>
     <sortCondition ref="B1:B1645"/>

</xml_diff>

<commit_message>
all programs, all subjects API
</commit_message>
<xml_diff>
--- a/sponsored_2018.xlsx
+++ b/sponsored_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Norman\Desktop\zagsabroad\zags-abroad-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57BF9914-2081-4618-9520-2AFF13D62E13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1345275-5735-4878-A29A-BC591E42FB24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="7425" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14663" windowHeight="8535" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL EQUIVALENCIES use Filter " sheetId="1" r:id="rId1"/>
@@ -21,10 +21,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL EQUIVALENCIES use Filter '!$K$1:$K$1447</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -57422,7 +57428,7 @@
     </row>
   </sheetData>
   <autoFilter ref="K1:K1447" xr:uid="{6DD63BD1-B5FC-4FFB-AEE6-8F2876966816}"/>
-  <sortState ref="A1:K1645">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:K1645">
     <sortCondition ref="A1:A1645"/>
     <sortCondition ref="B1:B1645"/>
   </sortState>
@@ -58284,7 +58290,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
adding the core designations
</commit_message>
<xml_diff>
--- a/sponsored_2018.xlsx
+++ b/sponsored_2018.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\OneDrive - Gonzaga University\Fall 2018\Senior Design\zags-abroad-backend\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Norman\Desktop\zagsabroad\zags-abroad-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A245E5F-9B24-4DF0-A9BA-B79B25FAA3F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF112A9F-CDA2-47CF-A5C2-40831E118422}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5078" windowHeight="8535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5078" windowHeight="8535" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL EQUIVALENCIES use Filter " sheetId="1" r:id="rId1"/>
     <sheet name="Programs" sheetId="2" r:id="rId2"/>
     <sheet name="Subjects" sheetId="3" r:id="rId3"/>
     <sheet name="Departments" sheetId="4" r:id="rId4"/>
+    <sheet name="CORE" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALL EQUIVALENCIES use Filter '!$L$1:$L$1447</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11762" uniqueCount="3801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11778" uniqueCount="3815">
   <si>
     <t>ART 5450</t>
   </si>
@@ -11453,12 +11454,54 @@
       <t xml:space="preserve"> ** CIVIL MAJORS ONLY</t>
     </r>
   </si>
+  <si>
+    <t>CHRISTIANITY AND CATHOLIC STUDIES</t>
+  </si>
+  <si>
+    <t>COMMUNICATION AND SPEECH</t>
+  </si>
+  <si>
+    <t>ETHICS</t>
+  </si>
+  <si>
+    <t>FINE ARTS</t>
+  </si>
+  <si>
+    <t>LITERATURE</t>
+  </si>
+  <si>
+    <t>PHILOSOPHY OF HUMAN NATURE</t>
+  </si>
+  <si>
+    <t>REASONING</t>
+  </si>
+  <si>
+    <t>SCIENTIFIC INQUIRY</t>
+  </si>
+  <si>
+    <t>SOCIAL AND BEHAVIORAL SCIENCES</t>
+  </si>
+  <si>
+    <t>WORLD OR COMPARATIVE RELIGION</t>
+  </si>
+  <si>
+    <t>WRITING</t>
+  </si>
+  <si>
+    <t>GLOBAL STUDIES DESIGNATION</t>
+  </si>
+  <si>
+    <t>SOCIAL JUSTICE DESIGNATION</t>
+  </si>
+  <si>
+    <t>WRITING ENRICHED DESIGNATION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11545,6 +11588,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -11613,7 +11664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -11715,6 +11766,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11998,7 +12050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C955" sqref="C955"/>
     </sheetView>
   </sheetViews>
@@ -58919,7 +58971,7 @@
     </row>
   </sheetData>
   <autoFilter ref="L1:L1447" xr:uid="{6DD63BD1-B5FC-4FFB-AEE6-8F2876966816}"/>
-  <sortState ref="A1:L1645">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:L1645">
     <sortCondition ref="A1:A1645"/>
     <sortCondition ref="B1:B1645"/>
   </sortState>
@@ -59131,8 +59183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA4B077-2B21-4097-A131-F4C3C7A92D62}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -59143,10 +59195,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="63" t="s">
         <v>3590</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="63" t="s">
         <v>3736</v>
       </c>
     </row>
@@ -59776,6 +59828,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -60350,4 +60403,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0EDF9D-9B19-44C6-BF6F-C94909280414}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="35.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>